<commit_message>
created new package for files
</commit_message>
<xml_diff>
--- a/PlateData/template.xlsx
+++ b/PlateData/template.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E79BF862-9FAC-4987-AB19-51DAB5EEADC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A63F5031-B11F-4D4A-AD85-0E27D2D07B82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="14196" windowHeight="13224" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <oleSize ref="A1:Q7"/>
+  <oleSize ref="A19:Q31"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1419,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2191,7 +2191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>